<commit_message>
added comments to export & to payment_add_form
</commit_message>
<xml_diff>
--- a/files/export.xlsx
+++ b/files/export.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Художник</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Алексеева Анастасия</t>
+  </si>
+  <si>
+    <t>2011-Sep-13 / 15:09</t>
   </si>
   <si>
     <t>10 / 23 см / картинка</t>
@@ -543,11 +546,11 @@
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3">
-        <v>1315912730</v>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -561,13 +564,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1315914153</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
export materials released + download fix
</commit_message>
<xml_diff>
--- a/files/export.xlsx
+++ b/files/export.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Художники" sheetId="1" r:id="rId4"/>
     <sheet name="Изделия" sheetId="2" r:id="rId5"/>
-    <sheet name="Платежи" sheetId="3" r:id="rId6"/>
+    <sheet name="Заготовки" sheetId="3" r:id="rId6"/>
+    <sheet name="Платежи" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="342">
   <si>
     <t>Художник</t>
   </si>
@@ -886,6 +887,102 @@
     <t>узкий</t>
   </si>
   <si>
+    <t>Наименование</t>
+  </si>
+  <si>
+    <t>М-30 большая</t>
+  </si>
+  <si>
+    <t>М-30 пузатая бородатая</t>
+  </si>
+  <si>
+    <t>М-20 большая</t>
+  </si>
+  <si>
+    <t>М-20 пузатая</t>
+  </si>
+  <si>
+    <t>М-15 большая</t>
+  </si>
+  <si>
+    <t>М-15 пузатая</t>
+  </si>
+  <si>
+    <t>М-10 большая</t>
+  </si>
+  <si>
+    <t>М-10 пузатая</t>
+  </si>
+  <si>
+    <t>М-5 18 см</t>
+  </si>
+  <si>
+    <t>М-5 14 см</t>
+  </si>
+  <si>
+    <t>М-5 12 см</t>
+  </si>
+  <si>
+    <t>М-5 9см</t>
+  </si>
+  <si>
+    <t>М-3 14 см</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> М-3 9 см</t>
+  </si>
+  <si>
+    <t>Колокольчик малый</t>
+  </si>
+  <si>
+    <t>Колокольчик большой</t>
+  </si>
+  <si>
+    <t>Яйцо</t>
+  </si>
+  <si>
+    <t>Шар малый</t>
+  </si>
+  <si>
+    <t>Шар большой</t>
+  </si>
+  <si>
+    <t>Неваляшка</t>
+  </si>
+  <si>
+    <t>Футляр 0,05</t>
+  </si>
+  <si>
+    <t>куколка сарафан</t>
+  </si>
+  <si>
+    <t>Яблоко</t>
+  </si>
+  <si>
+    <t>Груша</t>
+  </si>
+  <si>
+    <t>Браслет 1</t>
+  </si>
+  <si>
+    <t>Браслет 2</t>
+  </si>
+  <si>
+    <t>Браслет 3</t>
+  </si>
+  <si>
+    <t>Браслет 4</t>
+  </si>
+  <si>
+    <t>Браслет 5</t>
+  </si>
+  <si>
+    <t>Браслет 6</t>
+  </si>
+  <si>
+    <t>--Выберите заготовку--</t>
+  </si>
+  <si>
     <t>Мастер</t>
   </si>
   <si>
@@ -925,16 +1022,28 @@
     <t>7 / оформление / оформление</t>
   </si>
   <si>
-    <t>2011-Sep-23 / 01:09</t>
-  </si>
-  <si>
-    <t>15 / пузатая / картинка</t>
-  </si>
-  <si>
-    <t>2011-Sep-26 / 00:09</t>
-  </si>
-  <si>
-    <t>10 / 14 см / Жостово</t>
+    <t>2011-Sep-23 / 12:09</t>
+  </si>
+  <si>
+    <t>15 / пузатая / лицо</t>
+  </si>
+  <si>
+    <t>фы</t>
+  </si>
+  <si>
+    <t>2011-Sep-27 / 21:09</t>
+  </si>
+  <si>
+    <t>15 / большая / картинка</t>
+  </si>
+  <si>
+    <t>первый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ангел  / ангел  / ангел </t>
+  </si>
+  <si>
+    <t>второй</t>
   </si>
 </sst>
 </file>
@@ -6441,6 +6550,198 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
+  <dimension ref="A1:A33"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
@@ -6458,25 +6759,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>289</v>
+        <v>321</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>291</v>
+        <v>323</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>292</v>
+        <v>324</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>197</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -6484,10 +6785,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>295</v>
+        <v>327</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="D2" s="4">
         <v>3</v>
@@ -6507,10 +6808,10 @@
         <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>295</v>
+        <v>327</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -6530,10 +6831,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>295</v>
+        <v>327</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -6553,10 +6854,10 @@
         <v>184</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>298</v>
+        <v>330</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="D5" s="4">
         <v>2</v>
@@ -6574,10 +6875,10 @@
         <v>184</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>298</v>
+        <v>330</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -6586,7 +6887,7 @@
         <v>1400</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>300</v>
+        <v>332</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -6597,10 +6898,10 @@
         <v>88</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>298</v>
+        <v>330</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="D7" s="4">
         <v>2</v>
@@ -6609,7 +6910,7 @@
         <v>1560</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>300</v>
+        <v>332</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -6617,22 +6918,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>302</v>
+        <v>334</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>303</v>
+        <v>335</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
       </c>
       <c r="E8" s="4">
-        <v>2800</v>
+        <v>600</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>300</v>
+        <v>336</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -6643,39 +6944,43 @@
         <v>170</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="4">
-        <v>450</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>1750</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>339</v>
+      </c>
       <c r="G9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>303</v>
+        <v>340</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="4">
-        <v>1400</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="G10" s="4">
         <v>0</v>
       </c>

</xml_diff>